<commit_message>
Began dir and indir effects modeling
</commit_message>
<xml_diff>
--- a/data/cristageone.cur1.xlsx
+++ b/data/cristageone.cur1.xlsx
@@ -2230,10 +2230,10 @@
   <dimension ref="A1:EP91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="EB59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="EA47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EQ69" sqref="EQ69"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -29867,333 +29867,432 @@
       <c r="D69" s="2">
         <v>0</v>
       </c>
-      <c r="E69" s="3"/>
+      <c r="E69" s="3">
+        <v>-6.0999999999999943E-2</v>
+      </c>
       <c r="F69" s="3">
         <v>0.93899999999999995</v>
       </c>
       <c r="G69" s="2">
         <v>1</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3">
+        <v>-8.0000000000000071E-3</v>
+      </c>
       <c r="I69" s="3">
         <v>1.0109999999999999</v>
       </c>
       <c r="J69" s="2">
         <v>0</v>
       </c>
-      <c r="K69" s="3"/>
+      <c r="K69" s="3">
+        <v>1.0000000000000009E-2</v>
+      </c>
       <c r="L69" s="3">
         <v>0.93100000000000005</v>
       </c>
       <c r="M69" s="2">
         <v>1</v>
       </c>
-      <c r="N69" s="3"/>
+      <c r="N69" s="3">
+        <v>-1.3999999999999901E-2</v>
+      </c>
       <c r="O69" s="3">
         <v>1.0229999999999999</v>
       </c>
       <c r="P69" s="2">
         <v>0</v>
       </c>
-      <c r="Q69" s="3"/>
+      <c r="Q69" s="3">
+        <v>-5.600000000000005E-2</v>
+      </c>
       <c r="R69" s="3">
         <v>0.97199999999999998</v>
       </c>
       <c r="S69" s="2">
         <v>0</v>
       </c>
-      <c r="T69" s="3"/>
+      <c r="T69" s="3">
+        <v>4.0000000000000036E-3</v>
+      </c>
       <c r="U69" s="3">
         <v>0.94</v>
       </c>
       <c r="V69" s="2">
         <v>1</v>
       </c>
-      <c r="W69" s="3"/>
+      <c r="W69" s="3">
+        <v>-4.0000000000000036E-3</v>
+      </c>
       <c r="X69" s="3">
         <v>1.006</v>
       </c>
       <c r="Y69" s="2">
         <v>0</v>
       </c>
-      <c r="Z69" s="3"/>
+      <c r="Z69" s="3">
+        <v>3.400000000000003E-2</v>
+      </c>
       <c r="AA69" s="3">
         <v>1.0109999999999999</v>
       </c>
       <c r="AB69" s="2">
         <v>0</v>
       </c>
-      <c r="AC69" s="3"/>
+      <c r="AC69" s="3">
+        <v>1.0999999999999899E-2</v>
+      </c>
       <c r="AD69" s="3">
         <v>1.0009999999999999</v>
       </c>
       <c r="AE69" s="2">
         <v>0</v>
       </c>
-      <c r="AF69" s="3"/>
+      <c r="AF69" s="3">
+        <v>8.999999999999897E-3</v>
+      </c>
       <c r="AG69" s="3">
         <v>0.92900000000000005</v>
       </c>
       <c r="AH69" s="2">
         <v>1</v>
       </c>
-      <c r="AI69" s="3"/>
+      <c r="AI69" s="3">
+        <v>-1.4999999999999902E-2</v>
+      </c>
       <c r="AJ69" s="3">
         <v>0.98599999999999999</v>
       </c>
       <c r="AK69" s="2">
         <v>0</v>
       </c>
-      <c r="AL69" s="3"/>
+      <c r="AL69" s="3">
+        <v>1.7000000000000015E-2</v>
+      </c>
       <c r="AM69" s="3">
         <v>1.03</v>
       </c>
       <c r="AN69" s="2">
         <v>0</v>
       </c>
-      <c r="AO69" s="3"/>
+      <c r="AO69" s="3">
+        <v>-3.6999999999999922E-2</v>
+      </c>
       <c r="AP69" s="3">
         <v>1.0009999999999999</v>
       </c>
       <c r="AQ69" s="2">
         <v>0</v>
       </c>
-      <c r="AR69" s="3"/>
+      <c r="AR69" s="3">
+        <v>-4.1000000000000147E-2</v>
+      </c>
       <c r="AS69" s="3">
         <v>0.95399999999999996</v>
       </c>
       <c r="AT69" s="2">
         <v>1</v>
       </c>
-      <c r="AU69" s="3"/>
+      <c r="AU69" s="3">
+        <v>3.2999999999999918E-2</v>
+      </c>
       <c r="AV69" s="3">
         <v>0.98599999999999999</v>
       </c>
       <c r="AW69" s="2">
         <v>0</v>
       </c>
-      <c r="AX69" s="3"/>
+      <c r="AX69" s="3">
+        <v>-3.400000000000003E-2</v>
+      </c>
       <c r="AY69" s="3">
         <v>1.0129999999999999</v>
       </c>
       <c r="AZ69" s="2">
         <v>0</v>
       </c>
-      <c r="BA69" s="3"/>
+      <c r="BA69" s="3">
+        <v>1.0999999999999899E-2</v>
+      </c>
       <c r="BB69" s="3">
         <v>0.998</v>
       </c>
       <c r="BC69" s="2">
         <v>0</v>
       </c>
-      <c r="BD69" s="3"/>
+      <c r="BD69" s="3">
+        <v>-1.0000000000000009E-3</v>
+      </c>
       <c r="BE69" s="3">
         <v>0.94299999999999995</v>
       </c>
       <c r="BF69" s="2">
         <v>1</v>
       </c>
-      <c r="BG69" s="3"/>
+      <c r="BG69" s="3">
+        <v>1.2999999999999901E-2</v>
+      </c>
       <c r="BH69" s="3">
         <v>0.98899999999999999</v>
       </c>
       <c r="BI69" s="2">
         <v>0</v>
       </c>
-      <c r="BJ69" s="3"/>
+      <c r="BJ69" s="3">
+        <v>-2.300000000000002E-2</v>
+      </c>
       <c r="BK69" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="BL69" s="2">
         <v>1</v>
       </c>
-      <c r="BM69" s="3"/>
+      <c r="BM69" s="3">
+        <v>-4.3999999999999817E-2</v>
+      </c>
       <c r="BN69" s="3">
         <v>0.95799999999999996</v>
       </c>
       <c r="BO69" s="2">
         <v>1</v>
       </c>
-      <c r="BP69" s="3"/>
+      <c r="BP69" s="3">
+        <v>-3.5000000000000031E-2</v>
+      </c>
       <c r="BQ69" s="3">
         <v>1.046</v>
       </c>
       <c r="BR69" s="2">
         <v>1</v>
       </c>
-      <c r="BS69" s="3"/>
+      <c r="BS69" s="3">
+        <v>2.8000000000000025E-2</v>
+      </c>
       <c r="BT69" s="3">
         <v>1.0009999999999999</v>
       </c>
       <c r="BU69" s="2">
         <v>0</v>
       </c>
-      <c r="BV69" s="3"/>
+      <c r="BV69" s="3">
+        <v>-2.7000000000000135E-2</v>
+      </c>
       <c r="BW69" s="3">
         <v>0.97699999999999998</v>
       </c>
       <c r="BX69" s="2">
         <v>0</v>
       </c>
-      <c r="BY69" s="3"/>
+      <c r="BY69" s="3">
+        <v>2.1000000000000019E-2</v>
+      </c>
       <c r="BZ69" s="3">
         <v>1.0960000000000001</v>
       </c>
       <c r="CA69" s="2">
         <v>1</v>
       </c>
-      <c r="CB69" s="3"/>
+      <c r="CB69" s="3">
+        <v>-4.1999999999999815E-2</v>
+      </c>
       <c r="CC69" s="3">
         <v>1.022</v>
       </c>
       <c r="CD69" s="2">
         <v>0</v>
       </c>
-      <c r="CE69" s="3"/>
+      <c r="CE69" s="3">
+        <v>3.9000000000000035E-2</v>
+      </c>
       <c r="CF69" s="3">
         <v>1.0960000000000001</v>
       </c>
       <c r="CG69" s="2">
         <v>1</v>
       </c>
-      <c r="CH69" s="3"/>
+      <c r="CH69" s="3">
+        <v>0.10200000000000009</v>
+      </c>
       <c r="CI69" s="3">
         <v>1.0009999999999999</v>
       </c>
       <c r="CJ69" s="2">
         <v>0</v>
       </c>
-      <c r="CK69" s="3"/>
+      <c r="CK69" s="3">
+        <v>9.9999999999998979E-3</v>
+      </c>
       <c r="CL69" s="3">
         <v>1.046</v>
       </c>
       <c r="CM69" s="2">
         <v>1</v>
       </c>
-      <c r="CN69" s="3"/>
+      <c r="CN69" s="3">
+        <v>2.7000000000000135E-2</v>
+      </c>
       <c r="CO69" s="3">
         <v>1.0089999999999999</v>
       </c>
       <c r="CP69" s="2">
         <v>0</v>
       </c>
-      <c r="CQ69" s="3"/>
+      <c r="CQ69" s="3">
+        <v>3.499999999999992E-2</v>
+      </c>
       <c r="CR69" s="3">
         <v>1.002</v>
       </c>
-      <c r="CT69" s="3"/>
+      <c r="CS69" s="2">
+        <v>0</v>
+      </c>
+      <c r="CT69" s="3">
+        <v>-2.6999999999999913E-2</v>
+      </c>
       <c r="CU69" s="3">
         <v>0.96799999999999997</v>
       </c>
       <c r="CV69" s="2">
         <v>1</v>
       </c>
-      <c r="CW69" s="3"/>
+      <c r="CW69" s="3">
+        <v>-4.4999999999999929E-2</v>
+      </c>
       <c r="CX69" s="3">
         <v>1.1459999999999999</v>
       </c>
       <c r="CY69" s="2">
         <v>1</v>
       </c>
-      <c r="CZ69" s="3"/>
+      <c r="CZ69" s="3">
+        <v>1.8000000000000016E-2</v>
+      </c>
       <c r="DA69" s="3">
         <v>0.96599999999999997</v>
       </c>
       <c r="DB69" s="2">
         <v>1</v>
       </c>
-      <c r="DC69" s="3"/>
+      <c r="DC69" s="3">
+        <v>-8.0000000000000071E-3</v>
+      </c>
       <c r="DD69" s="3">
         <v>1.0149999999999999</v>
       </c>
       <c r="DE69" s="2">
         <v>0</v>
       </c>
-      <c r="DF69" s="3"/>
+      <c r="DF69" s="3">
+        <v>-2.100000000000013E-2</v>
+      </c>
       <c r="DG69" s="3">
         <v>0.97799999999999998</v>
       </c>
       <c r="DH69" s="2">
         <v>1</v>
       </c>
-      <c r="DI69" s="3"/>
+      <c r="DI69" s="3">
+        <v>-6.0000000000000053E-3</v>
+      </c>
       <c r="DJ69" s="3">
         <v>1.079</v>
       </c>
       <c r="DK69" s="2">
         <v>1</v>
       </c>
-      <c r="DL69" s="3"/>
+      <c r="DL69" s="3">
+        <v>3.6999999999999922E-2</v>
+      </c>
       <c r="DM69" s="3">
         <v>0.93300000000000005</v>
       </c>
       <c r="DN69" s="2">
         <v>1</v>
       </c>
-      <c r="DO69" s="3"/>
+      <c r="DO69" s="3">
+        <v>1.100000000000001E-2</v>
+      </c>
       <c r="DP69" s="3">
         <v>1.1279999999999999</v>
       </c>
       <c r="DQ69" s="2">
         <v>1</v>
       </c>
-      <c r="DR69" s="3"/>
+      <c r="DR69" s="3">
+        <v>-5.2000000000000046E-2</v>
+      </c>
       <c r="DS69" s="3">
         <v>1.103</v>
       </c>
       <c r="DT69" s="2">
         <v>1</v>
       </c>
-      <c r="DU69" s="3"/>
+      <c r="DU69" s="3">
+        <v>-7.0000000000001172E-3</v>
+      </c>
       <c r="DV69" s="3">
         <v>1.0349999999999999</v>
       </c>
       <c r="DW69" s="2">
         <v>0</v>
       </c>
-      <c r="DX69" s="3"/>
+      <c r="DX69" s="3">
+        <v>-0.12800000000000011</v>
+      </c>
       <c r="DY69" s="3">
         <v>0.98299999999999998</v>
       </c>
       <c r="DZ69" s="2">
         <v>0</v>
       </c>
-      <c r="EA69" s="3"/>
+      <c r="EA69" s="3">
+        <v>4.7999999999999932E-2</v>
+      </c>
       <c r="EB69" s="3">
         <v>0.94299999999999995</v>
       </c>
       <c r="EC69" s="2">
         <v>1</v>
       </c>
-      <c r="ED69" s="3"/>
+      <c r="ED69" s="3">
+        <v>-8.5999999999999965E-2</v>
+      </c>
       <c r="EE69" s="3">
         <v>1.0449999999999999</v>
       </c>
       <c r="EF69" s="2">
         <v>1</v>
       </c>
-      <c r="EG69" s="3"/>
+      <c r="EG69" s="3">
+        <v>4.9999999999999933E-2</v>
+      </c>
       <c r="EH69" s="3">
         <v>1.0049999999999999</v>
       </c>
       <c r="EI69" s="2">
         <v>0</v>
       </c>
-      <c r="EJ69" s="3"/>
+      <c r="EJ69" s="3">
+        <v>-1.5000000000000124E-2</v>
+      </c>
       <c r="EK69" s="3">
         <v>1.0409999999999999</v>
       </c>
       <c r="EL69" s="2">
         <v>1</v>
       </c>
-      <c r="EM69" s="3"/>
+      <c r="EM69" s="3">
+        <v>0.13099999999999989</v>
+      </c>
       <c r="EN69" s="3">
         <v>0.92200000000000004</v>
       </c>
       <c r="EO69" s="2">
         <v>1</v>
       </c>
-      <c r="EP69" s="3"/>
+      <c r="EP69" s="3">
+        <v>-0.16600000000000004</v>
+      </c>
     </row>
     <row r="70" spans="1:146" x14ac:dyDescent="0.25">
       <c r="A70" s="2">

</xml_diff>

<commit_message>
Anonymized team numbers added Code updates Half of anonymized code now shared
</commit_message>
<xml_diff>
--- a/data/cristageone.cur1.xlsx
+++ b/data/cristageone.cur1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5496"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2186,160 +2186,160 @@
   <dimension ref="A1:EP91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="EC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EQ1" sqref="EQ1:ES1048576"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="3"/>
-    <col min="4" max="4" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="3"/>
-    <col min="7" max="7" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="3"/>
-    <col min="10" max="10" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="3"/>
-    <col min="13" max="13" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="3"/>
-    <col min="16" max="16" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" style="3"/>
-    <col min="19" max="19" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.109375" style="3"/>
-    <col min="22" max="22" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" style="3"/>
-    <col min="25" max="25" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" style="3"/>
-    <col min="28" max="28" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.109375" style="4"/>
-    <col min="31" max="31" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.109375" style="4"/>
-    <col min="34" max="34" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.109375" style="4"/>
-    <col min="37" max="37" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.109375" style="4"/>
-    <col min="40" max="40" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.109375" style="4"/>
-    <col min="43" max="43" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.109375" style="4"/>
-    <col min="46" max="46" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.109375" style="4"/>
-    <col min="52" max="52" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.109375" style="4"/>
-    <col min="58" max="58" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.109375" style="4"/>
-    <col min="64" max="64" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="9.109375" style="4"/>
-    <col min="67" max="67" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9.109375" style="4"/>
-    <col min="70" max="70" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="9.109375" style="4"/>
-    <col min="73" max="73" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.109375" style="4"/>
-    <col min="76" max="76" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.109375" style="4"/>
-    <col min="79" max="79" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="9.109375" style="4"/>
-    <col min="82" max="82" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="9.109375" style="4"/>
-    <col min="85" max="85" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="9.109375" style="4"/>
-    <col min="88" max="88" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="9.109375" style="4"/>
-    <col min="91" max="91" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="9.109375" style="4"/>
-    <col min="94" max="94" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="9.109375" style="4"/>
-    <col min="97" max="97" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="9.109375" style="4"/>
-    <col min="100" max="100" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="9.109375" style="4"/>
-    <col min="103" max="103" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="9.109375" style="4"/>
-    <col min="106" max="106" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="9.109375" style="4"/>
-    <col min="109" max="109" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="9.109375" style="4"/>
-    <col min="112" max="112" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="9.109375" style="4"/>
-    <col min="115" max="115" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="9.109375" style="4"/>
-    <col min="118" max="118" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="9.109375" style="4"/>
-    <col min="121" max="121" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="9.109375" style="4"/>
-    <col min="124" max="124" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="9.109375" style="4"/>
-    <col min="127" max="127" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="9.109375" style="4"/>
-    <col min="130" max="130" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="9.109375" style="4"/>
-    <col min="133" max="133" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="9.109375" style="4"/>
-    <col min="136" max="136" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="9.109375" style="4"/>
-    <col min="139" max="139" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="9.109375" style="4"/>
-    <col min="142" max="142" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="9.109375" style="4"/>
-    <col min="145" max="145" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="147" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="2" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" style="3"/>
+    <col min="4" max="4" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" style="3"/>
+    <col min="7" max="7" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" style="3"/>
+    <col min="10" max="10" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.08984375" style="3"/>
+    <col min="13" max="13" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.08984375" style="3"/>
+    <col min="16" max="16" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.08984375" style="3"/>
+    <col min="19" max="19" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.08984375" style="3"/>
+    <col min="22" max="22" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.08984375" style="3"/>
+    <col min="25" max="25" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.08984375" style="3"/>
+    <col min="28" max="28" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.08984375" style="4"/>
+    <col min="31" max="31" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.08984375" style="4"/>
+    <col min="34" max="34" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.08984375" style="4"/>
+    <col min="37" max="37" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.08984375" style="4"/>
+    <col min="40" max="40" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.08984375" style="4"/>
+    <col min="43" max="43" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.08984375" style="4"/>
+    <col min="46" max="46" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.08984375" style="4"/>
+    <col min="52" max="52" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.08984375" style="4"/>
+    <col min="58" max="58" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.08984375" style="4"/>
+    <col min="64" max="64" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9.08984375" style="4"/>
+    <col min="67" max="67" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9.08984375" style="4"/>
+    <col min="70" max="70" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="9.08984375" style="4"/>
+    <col min="73" max="73" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.08984375" style="4"/>
+    <col min="76" max="76" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.08984375" style="4"/>
+    <col min="79" max="79" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="9.08984375" style="4"/>
+    <col min="82" max="82" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9.08984375" style="4"/>
+    <col min="85" max="85" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="9.08984375" style="4"/>
+    <col min="88" max="88" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="9.08984375" style="4"/>
+    <col min="91" max="91" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="9.08984375" style="4"/>
+    <col min="94" max="94" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="9.08984375" style="4"/>
+    <col min="97" max="97" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="9.08984375" style="4"/>
+    <col min="100" max="100" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="9.08984375" style="4"/>
+    <col min="103" max="103" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="9.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="9.08984375" style="4"/>
+    <col min="106" max="106" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="9.08984375" style="4"/>
+    <col min="109" max="109" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="9.08984375" style="4"/>
+    <col min="112" max="112" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="9.08984375" style="4"/>
+    <col min="115" max="115" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="9.08984375" style="4"/>
+    <col min="118" max="118" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="9.08984375" style="4"/>
+    <col min="121" max="121" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="9.08984375" style="4"/>
+    <col min="124" max="124" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="9.08984375" style="4"/>
+    <col min="127" max="127" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="9.08984375" style="4"/>
+    <col min="130" max="130" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="9.08984375" style="4"/>
+    <col min="133" max="133" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="9.08984375" style="4"/>
+    <col min="136" max="136" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="9.08984375" style="4"/>
+    <col min="139" max="139" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="9.08984375" style="4"/>
+    <col min="142" max="142" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="9.08984375" style="4"/>
+    <col min="145" max="145" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="147" max="16384" width="9.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:146" s="8" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:146" s="8" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="2" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3171,7 +3171,7 @@
       <c r="EO2" s="6"/>
       <c r="EP2" s="3"/>
     </row>
-    <row r="3" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4051,9 +4051,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -4443,9 +4443,9 @@
       <c r="EO5" s="6"/>
       <c r="EP5" s="3"/>
     </row>
-    <row r="6" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -4835,9 +4835,9 @@
       <c r="EO6" s="6"/>
       <c r="EP6" s="3"/>
     </row>
-    <row r="7" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -5227,9 +5227,9 @@
       <c r="EO7" s="6"/>
       <c r="EP7" s="3"/>
     </row>
-    <row r="8" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -5598,9 +5598,9 @@
       <c r="EO8" s="6"/>
       <c r="EP8" s="3"/>
     </row>
-    <row r="9" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -5990,9 +5990,9 @@
       <c r="EO9" s="6"/>
       <c r="EP9" s="3"/>
     </row>
-    <row r="10" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -6430,9 +6430,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="11">
         <v>1</v>
@@ -6870,9 +6870,9 @@
         <v>-1.8000000000000016E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -7262,9 +7262,9 @@
       <c r="EO12" s="6"/>
       <c r="EP12" s="3"/>
     </row>
-    <row r="13" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -7654,9 +7654,9 @@
       <c r="EO13" s="6"/>
       <c r="EP13" s="3"/>
     </row>
-    <row r="14" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -8046,9 +8046,9 @@
       <c r="EO14" s="6"/>
       <c r="EP14" s="3"/>
     </row>
-    <row r="15" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -8438,9 +8438,9 @@
       <c r="EO15" s="6"/>
       <c r="EP15" s="3"/>
     </row>
-    <row r="16" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -8878,9 +8878,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -9318,9 +9318,9 @@
         <v>-1.0000000000001119E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -9758,9 +9758,9 @@
         <v>2.9999999999998916E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -10150,9 +10150,9 @@
       <c r="EO19" s="6"/>
       <c r="EP19" s="3"/>
     </row>
-    <row r="20" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -10590,9 +10590,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -10982,9 +10982,9 @@
       <c r="EO21" s="6"/>
       <c r="EP21" s="3"/>
     </row>
-    <row r="22" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -11422,9 +11422,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -11814,9 +11814,9 @@
       <c r="EO23" s="6"/>
       <c r="EP23" s="3"/>
     </row>
-    <row r="24" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -12206,9 +12206,9 @@
       <c r="EO24" s="6"/>
       <c r="EP24" s="3"/>
     </row>
-    <row r="25" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -12598,9 +12598,9 @@
       <c r="EO25" s="6"/>
       <c r="EP25" s="3"/>
     </row>
-    <row r="26" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -13038,9 +13038,9 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="27" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -13430,9 +13430,9 @@
       <c r="EO27" s="6"/>
       <c r="EP27" s="3"/>
     </row>
-    <row r="28" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -13822,9 +13822,9 @@
       <c r="EO28" s="6"/>
       <c r="EP28" s="3"/>
     </row>
-    <row r="29" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -14214,9 +14214,9 @@
       <c r="EO29" s="6"/>
       <c r="EP29" s="3"/>
     </row>
-    <row r="30" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -14654,9 +14654,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -15046,9 +15046,9 @@
       <c r="EO31" s="6"/>
       <c r="EP31" s="3"/>
     </row>
-    <row r="32" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -15486,9 +15486,9 @@
         <v>2.9999999999998916E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -15878,9 +15878,9 @@
       <c r="EO33" s="6"/>
       <c r="EP33" s="3"/>
     </row>
-    <row r="34" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -16270,9 +16270,9 @@
       <c r="EO34" s="6"/>
       <c r="EP34" s="3"/>
     </row>
-    <row r="35" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
@@ -16710,9 +16710,9 @@
         <v>1.2000000000000011E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -17102,9 +17102,9 @@
       <c r="EO36" s="6"/>
       <c r="EP36" s="3"/>
     </row>
-    <row r="37" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -17542,9 +17542,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -17982,9 +17982,9 @@
         <v>1.2000000000000011E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -18422,9 +18422,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -18862,9 +18862,9 @@
         <v>-1.7000000000000126E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -19302,9 +19302,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -19742,9 +19742,9 @@
         <v>0.16599999999999993</v>
       </c>
     </row>
-    <row r="43" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -20182,9 +20182,9 @@
         <v>2.0000000000000018E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -20566,9 +20566,9 @@
       <c r="EN44" s="3"/>
       <c r="EP44" s="3"/>
     </row>
-    <row r="45" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -21006,9 +21006,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -21446,9 +21446,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -21830,9 +21830,9 @@
       <c r="EN47" s="3"/>
       <c r="EP47" s="3"/>
     </row>
-    <row r="48" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -22270,9 +22270,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -22710,9 +22710,9 @@
         <v>-3.0000000000001137E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -23094,9 +23094,9 @@
       <c r="EN50" s="3"/>
       <c r="EP50" s="3"/>
     </row>
-    <row r="51" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -23478,9 +23478,9 @@
       <c r="EN51" s="3"/>
       <c r="EP51" s="3"/>
     </row>
-    <row r="52" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -23633,9 +23633,9 @@
       <c r="EN52" s="3"/>
       <c r="EP52" s="3"/>
     </row>
-    <row r="53" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B53" s="11">
         <v>0</v>
@@ -24025,9 +24025,9 @@
       <c r="EO53" s="10"/>
       <c r="EP53" s="12"/>
     </row>
-    <row r="54" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -24465,9 +24465,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -24849,9 +24849,9 @@
       <c r="EN55" s="3"/>
       <c r="EP55" s="3"/>
     </row>
-    <row r="56" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -25233,9 +25233,9 @@
       <c r="EN56" s="3"/>
       <c r="EP56" s="3"/>
     </row>
-    <row r="57" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -25673,9 +25673,9 @@
         <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -26057,9 +26057,9 @@
       <c r="EN58" s="3"/>
       <c r="EP58" s="3"/>
     </row>
-    <row r="59" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
@@ -26441,9 +26441,9 @@
       <c r="EN59" s="3"/>
       <c r="EP59" s="3"/>
     </row>
-    <row r="60" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
@@ -26825,9 +26825,9 @@
       <c r="EN60" s="3"/>
       <c r="EP60" s="3"/>
     </row>
-    <row r="61" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -27139,9 +27139,9 @@
       <c r="EN61" s="3"/>
       <c r="EP61" s="3"/>
     </row>
-    <row r="62" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
-        <v>71</v>
+        <v>710</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -27234,9 +27234,9 @@
       <c r="EN62" s="3"/>
       <c r="EP62" s="3"/>
     </row>
-    <row r="63" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -27674,9 +27674,9 @@
         <v>-6.2000000000000055E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -28114,9 +28114,9 @@
         <v>-3.0000000000001137E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
@@ -28498,9 +28498,9 @@
       <c r="EN65" s="3"/>
       <c r="EP65" s="3"/>
     </row>
-    <row r="66" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B66" s="1">
         <v>1</v>
@@ -28938,9 +28938,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
@@ -29378,9 +29378,9 @@
         <v>-1.0000000000001119E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B68" s="11">
         <v>1</v>
@@ -29818,9 +29818,9 @@
         <v>-1.5000000000000124E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B69" s="1">
         <v>1</v>
@@ -30258,9 +30258,9 @@
         <v>-0.16600000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:146" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:146" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -30642,9 +30642,9 @@
       <c r="EN70" s="3"/>
       <c r="EP70" s="3"/>
     </row>
-    <row r="71" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -31026,9 +31026,9 @@
       <c r="EN71" s="3"/>
       <c r="EP71" s="3"/>
     </row>
-    <row r="72" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -31410,9 +31410,9 @@
       <c r="EN72" s="3"/>
       <c r="EP72" s="3"/>
     </row>
-    <row r="73" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B73" s="11">
         <v>1</v>
@@ -31850,9 +31850,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B74" s="1">
         <v>1</v>
@@ -32290,9 +32290,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -32730,9 +32730,9 @@
         <v>-2.200000000000002E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B76" s="1">
         <v>1</v>
@@ -33170,9 +33170,9 @@
         <v>-1.0000000000001119E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B77" s="1">
         <v>0</v>
@@ -33554,9 +33554,9 @@
       <c r="EN77" s="3"/>
       <c r="EP77" s="3"/>
     </row>
-    <row r="78" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
@@ -33938,9 +33938,9 @@
       <c r="EN78" s="3"/>
       <c r="EP78" s="3"/>
     </row>
-    <row r="79" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B79" s="1">
         <v>1</v>
@@ -34378,9 +34378,9 @@
         <v>-1.0000000000001119E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="B80" s="1">
         <v>0</v>
@@ -34762,9 +34762,9 @@
       <c r="EN80" s="3"/>
       <c r="EP80" s="3"/>
     </row>
-    <row r="81" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1">
         <v>1</v>
@@ -35202,9 +35202,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1">
         <v>0</v>
@@ -35586,9 +35586,9 @@
       <c r="EN82" s="3"/>
       <c r="EP82" s="3"/>
     </row>
-    <row r="83" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B83" s="1">
         <v>0</v>
@@ -35970,9 +35970,9 @@
       <c r="EN83" s="3"/>
       <c r="EP83" s="3"/>
     </row>
-    <row r="84" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
@@ -36354,9 +36354,9 @@
       <c r="EN84" s="3"/>
       <c r="EP84" s="3"/>
     </row>
-    <row r="85" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B85" s="1">
         <v>0</v>
@@ -36738,9 +36738,9 @@
       <c r="EN85" s="3"/>
       <c r="EP85" s="3"/>
     </row>
-    <row r="86" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B86" s="1">
         <v>1</v>
@@ -37178,9 +37178,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B87" s="1">
         <v>0</v>
@@ -37562,9 +37562,9 @@
       <c r="EN87" s="3"/>
       <c r="EP87" s="3"/>
     </row>
-    <row r="88" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
@@ -37946,9 +37946,9 @@
       <c r="EN88" s="3"/>
       <c r="EP88" s="3"/>
     </row>
-    <row r="89" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B89" s="1">
         <v>0</v>
@@ -38330,7 +38330,7 @@
       <c r="EN89" s="3"/>
       <c r="EP89" s="3"/>
     </row>
-    <row r="90" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>200</v>
       </c>
@@ -38770,7 +38770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:146" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>300</v>
       </c>
@@ -39155,7 +39155,7 @@
       <c r="EP91" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:EP92">
+  <sortState ref="A2:ER92">
     <sortCondition descending="1" ref="B2:B92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed team 70 results copy/paste error
</commit_message>
<xml_diff>
--- a/data/cristageone.cur1.xlsx
+++ b/data/cristageone.cur1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3761" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3789" uniqueCount="598">
   <si>
     <t>Team ID</t>
   </si>
@@ -2186,10 +2186,10 @@
   <dimension ref="A1:EP91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:C1048576"/>
+      <selection pane="bottomRight" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -31410,443 +31410,443 @@
       <c r="EN72" s="3"/>
       <c r="EP72" s="3"/>
     </row>
-    <row r="73" spans="1:146" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="10">
+    <row r="73" spans="1:146" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
         <v>70</v>
       </c>
-      <c r="B73" s="11">
-        <v>1</v>
-      </c>
-      <c r="C73" s="12" t="s">
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="10">
-        <v>1</v>
-      </c>
-      <c r="E73" s="12">
-        <v>0</v>
-      </c>
-      <c r="F73" s="12" t="s">
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G73" s="10">
-        <v>1</v>
-      </c>
-      <c r="H73" s="12">
-        <v>0</v>
-      </c>
-      <c r="I73" s="12" t="s">
+      <c r="G73" s="2">
+        <v>1</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J73" s="10">
-        <v>0</v>
-      </c>
-      <c r="K73" s="12">
-        <v>0</v>
-      </c>
-      <c r="L73" s="12" t="s">
+      <c r="J73" s="2">
+        <v>0</v>
+      </c>
+      <c r="K73" s="3">
+        <v>0</v>
+      </c>
+      <c r="L73" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M73" s="10">
-        <v>1</v>
-      </c>
-      <c r="N73" s="12">
-        <v>0</v>
-      </c>
-      <c r="O73" s="12" t="s">
+      <c r="M73" s="2">
+        <v>1</v>
+      </c>
+      <c r="N73" s="3">
+        <v>0</v>
+      </c>
+      <c r="O73" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P73" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="12">
-        <v>0</v>
-      </c>
-      <c r="R73" s="12" t="s">
+      <c r="P73" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="3">
+        <v>0</v>
+      </c>
+      <c r="R73" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="S73" s="10">
-        <v>0</v>
-      </c>
-      <c r="T73" s="12">
-        <v>0</v>
-      </c>
-      <c r="U73" s="12" t="s">
+      <c r="S73" s="2">
+        <v>0</v>
+      </c>
+      <c r="T73" s="3">
+        <v>0</v>
+      </c>
+      <c r="U73" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="V73" s="10">
-        <v>1</v>
-      </c>
-      <c r="W73" s="12">
-        <v>0</v>
-      </c>
-      <c r="X73" s="12" t="s">
+      <c r="V73" s="2">
+        <v>1</v>
+      </c>
+      <c r="W73" s="3">
+        <v>0</v>
+      </c>
+      <c r="X73" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Y73" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AA73" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB73" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD73" s="12" t="s">
+      <c r="Y73" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA73" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB73" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD73" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AE73" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AG73" s="12" t="s">
+      <c r="AE73" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG73" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AH73" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AJ73" s="12" t="s">
+      <c r="AH73" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AK73" s="10">
-        <v>0</v>
-      </c>
-      <c r="AL73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AM73" s="12" t="s">
+      <c r="AK73" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM73" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AN73" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AP73" s="12" t="s">
+      <c r="AN73" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP73" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AQ73" s="10">
-        <v>0</v>
-      </c>
-      <c r="AR73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AS73" s="12" t="s">
+      <c r="AQ73" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS73" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AT73" s="10">
-        <v>1</v>
-      </c>
-      <c r="AU73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AV73" s="12" t="s">
+      <c r="AT73" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV73" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AW73" s="10">
-        <v>1</v>
-      </c>
-      <c r="AX73" s="12">
-        <v>0</v>
-      </c>
-      <c r="AY73" s="12" t="s">
+      <c r="AW73" s="2">
+        <v>1</v>
+      </c>
+      <c r="AX73" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY73" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AZ73" s="10">
-        <v>0</v>
-      </c>
-      <c r="BA73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BB73" s="12" t="s">
+      <c r="AZ73" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB73" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="BC73" s="10">
-        <v>0</v>
-      </c>
-      <c r="BD73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BE73" s="12" t="s">
+      <c r="BC73" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BE73" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BF73" s="10">
-        <v>1</v>
-      </c>
-      <c r="BG73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BH73" s="12" t="s">
+      <c r="BF73" s="2">
+        <v>1</v>
+      </c>
+      <c r="BG73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BH73" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="BI73" s="10">
-        <v>0</v>
-      </c>
-      <c r="BJ73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BK73" s="12">
-        <v>1.1439999999999999</v>
-      </c>
-      <c r="BL73" s="10">
-        <v>1</v>
-      </c>
-      <c r="BM73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BN73" s="12">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="BO73" s="10">
-        <v>1</v>
-      </c>
-      <c r="BP73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BQ73" s="12">
-        <v>1.018</v>
-      </c>
-      <c r="BR73" s="10">
-        <v>0</v>
-      </c>
-      <c r="BS73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BT73" s="12">
-        <v>1.028</v>
-      </c>
-      <c r="BU73" s="10">
-        <v>0</v>
-      </c>
-      <c r="BV73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BW73" s="12">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="BX73" s="10">
-        <v>1</v>
-      </c>
-      <c r="BY73" s="12">
-        <v>0</v>
-      </c>
-      <c r="BZ73" s="12">
-        <v>1.1379999999999999</v>
-      </c>
-      <c r="CA73" s="10">
-        <v>1</v>
-      </c>
-      <c r="CB73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CC73" s="12">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="CD73" s="10">
-        <v>0</v>
-      </c>
-      <c r="CE73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CF73" s="12">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="CG73" s="10">
-        <v>1</v>
-      </c>
-      <c r="CH73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CI73" s="12">
-        <v>0.99099999999999999</v>
-      </c>
-      <c r="CJ73" s="10">
-        <v>0</v>
-      </c>
-      <c r="CK73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CL73" s="12">
-        <v>1.0189999999999999</v>
-      </c>
-      <c r="CM73" s="10">
-        <v>0</v>
-      </c>
-      <c r="CN73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CO73" s="12">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="CP73" s="10">
-        <v>0</v>
-      </c>
-      <c r="CQ73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CR73" s="12">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="CS73" s="10">
-        <v>0</v>
-      </c>
-      <c r="CT73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CU73" s="12">
-        <v>1.0129999999999999</v>
-      </c>
-      <c r="CV73" s="10">
-        <v>1</v>
-      </c>
-      <c r="CW73" s="12">
-        <v>0</v>
-      </c>
-      <c r="CX73" s="12">
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="CY73" s="10">
-        <v>1</v>
-      </c>
-      <c r="CZ73" s="12">
-        <v>0</v>
-      </c>
-      <c r="DA73" s="12">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="DB73" s="10">
-        <v>0</v>
-      </c>
-      <c r="DC73" s="12">
-        <v>0</v>
-      </c>
-      <c r="DD73" s="12">
-        <v>1.0089999999999999</v>
-      </c>
-      <c r="DE73" s="10">
-        <v>1</v>
-      </c>
-      <c r="DF73" s="12">
-        <v>-2.7000000000000135E-2</v>
-      </c>
-      <c r="DG73" s="12">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="DH73" s="10">
-        <v>1</v>
-      </c>
-      <c r="DI73" s="12">
-        <v>0</v>
-      </c>
-      <c r="DJ73" s="12">
-        <v>1.01</v>
-      </c>
-      <c r="DK73" s="10">
-        <v>0</v>
-      </c>
-      <c r="DL73" s="12">
-        <v>-3.2000000000000028E-2</v>
-      </c>
-      <c r="DM73" s="12">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="DN73" s="10">
-        <v>0</v>
-      </c>
-      <c r="DO73" s="12">
-        <v>0</v>
-      </c>
-      <c r="DP73" s="12">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="DQ73" s="10">
-        <v>0</v>
-      </c>
-      <c r="DR73" s="12">
-        <v>-0.19799999999999995</v>
-      </c>
-      <c r="DS73" s="12">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="DT73" s="10">
-        <v>0</v>
-      </c>
-      <c r="DU73" s="12">
-        <v>0</v>
-      </c>
-      <c r="DV73" s="12">
-        <v>1.163</v>
-      </c>
-      <c r="DW73" s="10">
-        <v>1</v>
-      </c>
-      <c r="DX73" s="12">
-        <v>0</v>
-      </c>
-      <c r="DY73" s="12">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="DZ73" s="10">
-        <v>1</v>
-      </c>
-      <c r="EA73" s="12">
-        <v>0</v>
-      </c>
-      <c r="EB73" s="12">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="EC73" s="10">
-        <v>1</v>
-      </c>
-      <c r="ED73" s="12">
-        <v>0</v>
-      </c>
-      <c r="EE73" s="12">
-        <v>0.995</v>
-      </c>
-      <c r="EF73" s="10">
-        <v>1</v>
-      </c>
-      <c r="EG73" s="12">
-        <v>0</v>
-      </c>
-      <c r="EH73" s="12">
-        <v>1.02</v>
-      </c>
-      <c r="EI73" s="10">
-        <v>0</v>
-      </c>
-      <c r="EJ73" s="12">
-        <v>0</v>
-      </c>
-      <c r="EK73" s="12">
-        <v>0.91</v>
-      </c>
-      <c r="EL73" s="10">
-        <v>0</v>
-      </c>
-      <c r="EM73" s="12">
-        <v>0</v>
-      </c>
-      <c r="EN73" s="12">
-        <v>1.0880000000000001</v>
-      </c>
-      <c r="EO73" s="10">
-        <v>0</v>
-      </c>
-      <c r="EP73" s="12">
+      <c r="BI73" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BK73" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL73" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BO73" s="2">
+        <v>0</v>
+      </c>
+      <c r="BP73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BQ73" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR73" s="2">
+        <v>0</v>
+      </c>
+      <c r="BS73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BT73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BU73" s="2">
+        <v>1</v>
+      </c>
+      <c r="BV73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW73" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="BX73" s="2">
+        <v>0</v>
+      </c>
+      <c r="BY73" s="3">
+        <v>0</v>
+      </c>
+      <c r="BZ73" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="CA73" s="2">
+        <v>1</v>
+      </c>
+      <c r="CB73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CC73" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="CD73" s="2">
+        <v>0</v>
+      </c>
+      <c r="CE73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CF73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="CG73" s="2">
+        <v>0</v>
+      </c>
+      <c r="CH73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CI73" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="CJ73" s="2">
+        <v>0</v>
+      </c>
+      <c r="CK73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CL73" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="CM73" s="2">
+        <v>0</v>
+      </c>
+      <c r="CN73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CO73" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="CP73" s="2">
+        <v>0</v>
+      </c>
+      <c r="CQ73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CR73" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="CS73" s="2">
+        <v>1</v>
+      </c>
+      <c r="CT73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CU73" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="CV73" s="2">
+        <v>0</v>
+      </c>
+      <c r="CW73" s="3">
+        <v>0</v>
+      </c>
+      <c r="CX73" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="CY73" s="2">
+        <v>1</v>
+      </c>
+      <c r="CZ73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DA73" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="DB73" s="2">
+        <v>1</v>
+      </c>
+      <c r="DC73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DD73" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="DE73" s="2">
+        <v>0</v>
+      </c>
+      <c r="DF73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DG73" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH73" s="2">
+        <v>0</v>
+      </c>
+      <c r="DI73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DJ73" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="DK73" s="2">
+        <v>0</v>
+      </c>
+      <c r="DL73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DM73" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="DN73" s="2">
+        <v>1</v>
+      </c>
+      <c r="DO73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DP73" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="DQ73" s="2">
+        <v>1</v>
+      </c>
+      <c r="DR73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DS73" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="DT73" s="2">
+        <v>1</v>
+      </c>
+      <c r="DU73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DV73" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="DW73" s="2">
+        <v>1</v>
+      </c>
+      <c r="DX73" s="3">
+        <v>0</v>
+      </c>
+      <c r="DY73" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="DZ73" s="2">
+        <v>1</v>
+      </c>
+      <c r="EA73" s="3">
+        <v>0</v>
+      </c>
+      <c r="EB73" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="EC73" s="2">
+        <v>0</v>
+      </c>
+      <c r="ED73" s="3">
+        <v>0</v>
+      </c>
+      <c r="EE73" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="EF73" s="2">
+        <v>0</v>
+      </c>
+      <c r="EG73" s="3">
+        <v>0</v>
+      </c>
+      <c r="EH73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="EI73" s="2">
+        <v>0</v>
+      </c>
+      <c r="EJ73" s="3">
+        <v>0</v>
+      </c>
+      <c r="EK73" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="EL73" s="2">
+        <v>1</v>
+      </c>
+      <c r="EM73" s="3">
+        <v>0</v>
+      </c>
+      <c r="EN73" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="EO73" s="2">
+        <v>1</v>
+      </c>
+      <c r="EP73" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>